<commit_message>
Reserved two IDs (200001, 200002)
</commit_message>
<xml_diff>
--- a/Material classification.xlsx
+++ b/Material classification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katja\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TCCMaterialLibrary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E6DEDB-34C2-428F-AACD-8F475CC1701F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A3B165-8846-4235-A2DE-214307272388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="816" activeTab="1" xr2:uid="{6F2A3154-DBF6-40E9-8E64-C416931478F8}"/>
+    <workbookView xWindow="5085" yWindow="1740" windowWidth="21600" windowHeight="11385" tabRatio="816" activeTab="1" xr2:uid="{6F2A3154-DBF6-40E9-8E64-C416931478F8}"/>
   </bookViews>
   <sheets>
     <sheet name="ID creation" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
   <si>
     <t>METALS AND ALLOYS</t>
   </si>
@@ -249,13 +249,87 @@
   </si>
   <si>
     <t>Emissivity at RT</t>
+  </si>
+  <si>
+    <r>
+      <t>LaCoO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>La</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sr</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CoO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +353,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -375,7 +457,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -396,7 +478,6 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -914,10 +995,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F6D9E-7E96-474D-8137-0B481F54EEF6}">
-  <dimension ref="A1:BH7"/>
+  <dimension ref="A1:BH9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AW14" sqref="AW14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1595,179 +1676,179 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:60" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>310001</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="18">
-        <v>0</v>
-      </c>
-      <c r="F6" s="18">
-        <v>0</v>
-      </c>
-      <c r="G6" s="18">
-        <v>0</v>
-      </c>
-      <c r="H6" s="18">
-        <v>1</v>
-      </c>
-      <c r="I6" s="18">
-        <v>0</v>
-      </c>
-      <c r="J6" s="18">
-        <v>0</v>
-      </c>
-      <c r="K6" s="18">
-        <v>0</v>
-      </c>
-      <c r="L6" s="18">
-        <v>0</v>
-      </c>
-      <c r="M6" s="18">
-        <v>0</v>
-      </c>
-      <c r="N6" s="18">
-        <v>1</v>
-      </c>
-      <c r="O6" s="18">
-        <v>1</v>
-      </c>
-      <c r="P6" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="18">
-        <v>1</v>
-      </c>
-      <c r="R6" s="18">
-        <v>1</v>
-      </c>
-      <c r="S6" s="18">
-        <v>1</v>
-      </c>
-      <c r="T6" s="18">
-        <v>0</v>
-      </c>
-      <c r="U6" s="18">
-        <v>0</v>
-      </c>
-      <c r="V6" s="18">
-        <v>0</v>
-      </c>
-      <c r="W6" s="18">
-        <v>0</v>
-      </c>
-      <c r="X6" s="18">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="18">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="18">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="18">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="18">
-        <v>1</v>
-      </c>
-      <c r="AG6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="18">
-        <v>1</v>
-      </c>
-      <c r="AK6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AO6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AP6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AS6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AT6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AU6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AV6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AW6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AX6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AY6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AZ6" s="18">
-        <v>0</v>
-      </c>
-      <c r="BA6" s="18">
-        <v>0</v>
-      </c>
-      <c r="BB6" s="18">
-        <v>0</v>
-      </c>
-      <c r="BC6" s="18">
-        <v>0</v>
-      </c>
-      <c r="BD6" s="18">
-        <v>0</v>
-      </c>
-      <c r="BE6" s="18">
-        <v>0</v>
-      </c>
-      <c r="BF6" s="18">
-        <v>0</v>
-      </c>
-      <c r="BG6" s="18">
-        <v>0</v>
-      </c>
-      <c r="BH6" s="18">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>1</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>0</v>
+      </c>
+      <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="AW6">
+        <v>0</v>
+      </c>
+      <c r="AX6">
+        <v>0</v>
+      </c>
+      <c r="AY6">
+        <v>0</v>
+      </c>
+      <c r="AZ6">
+        <v>0</v>
+      </c>
+      <c r="BA6">
+        <v>0</v>
+      </c>
+      <c r="BB6">
+        <v>0</v>
+      </c>
+      <c r="BC6">
+        <v>0</v>
+      </c>
+      <c r="BD6">
+        <v>0</v>
+      </c>
+      <c r="BE6">
+        <v>0</v>
+      </c>
+      <c r="BF6">
+        <v>0</v>
+      </c>
+      <c r="BG6">
+        <v>0</v>
+      </c>
+      <c r="BH6">
         <v>0</v>
       </c>
     </row>
@@ -1781,173 +1862,189 @@
       <c r="C7" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="18">
-        <v>1</v>
-      </c>
-      <c r="F7" s="18">
-        <v>0</v>
-      </c>
-      <c r="G7" s="18">
-        <v>0</v>
-      </c>
-      <c r="H7" s="18">
-        <v>0</v>
-      </c>
-      <c r="I7" s="18">
-        <v>0</v>
-      </c>
-      <c r="J7" s="18">
-        <v>0</v>
-      </c>
-      <c r="K7" s="18">
-        <v>0</v>
-      </c>
-      <c r="L7" s="18">
-        <v>0</v>
-      </c>
-      <c r="M7" s="18">
-        <v>0</v>
-      </c>
-      <c r="N7" s="18">
-        <v>1</v>
-      </c>
-      <c r="O7" s="18">
-        <v>1</v>
-      </c>
-      <c r="P7" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="18">
-        <v>1</v>
-      </c>
-      <c r="R7" s="18">
-        <v>1</v>
-      </c>
-      <c r="S7" s="18">
-        <v>0</v>
-      </c>
-      <c r="T7" s="18">
-        <v>0</v>
-      </c>
-      <c r="U7" s="18">
-        <v>0</v>
-      </c>
-      <c r="V7" s="18">
-        <v>0</v>
-      </c>
-      <c r="W7" s="18">
-        <v>0</v>
-      </c>
-      <c r="X7" s="18">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="18">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="18">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="18">
-        <v>1</v>
-      </c>
-      <c r="AB7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="18">
-        <v>1</v>
-      </c>
-      <c r="AF7" s="18">
-        <v>1</v>
-      </c>
-      <c r="AG7" s="18">
-        <v>1</v>
-      </c>
-      <c r="AH7" s="18">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AF7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AH7">
         <v>0</v>
       </c>
       <c r="AI7">
         <v>0</v>
       </c>
-      <c r="AJ7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AM7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AN7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AO7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AP7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AQ7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AS7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AT7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AU7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AV7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AW7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AX7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AY7" s="18">
-        <v>0</v>
-      </c>
-      <c r="AZ7" s="18">
-        <v>0</v>
-      </c>
-      <c r="BA7" s="18">
-        <v>0</v>
-      </c>
-      <c r="BB7" s="18">
-        <v>0</v>
-      </c>
-      <c r="BC7" s="18">
-        <v>0</v>
-      </c>
-      <c r="BD7" s="18">
-        <v>0</v>
-      </c>
-      <c r="BE7" s="18">
-        <v>0</v>
-      </c>
-      <c r="BF7" s="18">
-        <v>0</v>
-      </c>
-      <c r="BG7" s="18">
-        <v>0</v>
-      </c>
-      <c r="BH7" s="18">
-        <v>0</v>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AU7">
+        <v>0</v>
+      </c>
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="AW7">
+        <v>0</v>
+      </c>
+      <c r="AX7">
+        <v>0</v>
+      </c>
+      <c r="AY7">
+        <v>0</v>
+      </c>
+      <c r="AZ7">
+        <v>0</v>
+      </c>
+      <c r="BA7">
+        <v>0</v>
+      </c>
+      <c r="BB7">
+        <v>0</v>
+      </c>
+      <c r="BC7">
+        <v>0</v>
+      </c>
+      <c r="BD7">
+        <v>0</v>
+      </c>
+      <c r="BE7">
+        <v>0</v>
+      </c>
+      <c r="BF7">
+        <v>0</v>
+      </c>
+      <c r="BG7">
+        <v>0</v>
+      </c>
+      <c r="BH7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:60" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>200001</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:60" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>200002</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2020,16 +2117,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543E0AFA-6024-4581-9565-D9A221BC4139}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A4" sqref="A4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2054,8 +2151,25 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
     </row>
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>200001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>200002</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2095,48 +2209,35 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>310001</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated instructions, added subfolders. Added LaFeMnSi.
</commit_message>
<xml_diff>
--- a/Material classification.xlsx
+++ b/Material classification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TCCMaterialLibrary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A3B165-8846-4235-A2DE-214307272388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E28BF2-D3C0-4439-A02F-5EFA62D520E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="1740" windowWidth="21600" windowHeight="11385" tabRatio="816" activeTab="1" xr2:uid="{6F2A3154-DBF6-40E9-8E64-C416931478F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="816" activeTab="2" xr2:uid="{6F2A3154-DBF6-40E9-8E64-C416931478F8}"/>
   </bookViews>
   <sheets>
     <sheet name="ID creation" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="81">
   <si>
     <t>METALS AND ALLOYS</t>
   </si>
@@ -323,6 +323,27 @@
       </rPr>
       <t>3</t>
     </r>
+  </si>
+  <si>
+    <t>La0.7Sr0.3CoO3</t>
+  </si>
+  <si>
+    <t>LaSrCoO</t>
+  </si>
+  <si>
+    <t>LaCoO3</t>
+  </si>
+  <si>
+    <t>LaCoO</t>
+  </si>
+  <si>
+    <t>LaFeMnSiH</t>
+  </si>
+  <si>
+    <t>La(Fe-Mn0.06-Si)13-H</t>
+  </si>
+  <si>
+    <t>Alloy; variable Mn content</t>
   </si>
 </sst>
 </file>
@@ -995,18 +1016,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F6D9E-7E96-474D-8137-0B481F54EEF6}">
-  <dimension ref="A1:BH9"/>
+  <dimension ref="A1:BH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -2031,20 +2052,208 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:60" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>200001</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:60" ht="18" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>200002</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>100003</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>1</v>
+      </c>
+      <c r="AL10">
+        <v>1</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <v>1</v>
+      </c>
+      <c r="AO10">
+        <v>1</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
+      </c>
+      <c r="AS10">
+        <v>0</v>
+      </c>
+      <c r="AT10">
+        <v>0</v>
+      </c>
+      <c r="AU10">
+        <v>0</v>
+      </c>
+      <c r="AV10">
+        <v>0</v>
+      </c>
+      <c r="AW10">
+        <v>0</v>
+      </c>
+      <c r="AX10">
+        <v>0</v>
+      </c>
+      <c r="AY10">
+        <v>0</v>
+      </c>
+      <c r="AZ10">
+        <v>0</v>
+      </c>
+      <c r="BA10">
+        <v>0</v>
+      </c>
+      <c r="BB10">
+        <v>0</v>
+      </c>
+      <c r="BC10">
+        <v>0</v>
+      </c>
+      <c r="BD10">
+        <v>0</v>
+      </c>
+      <c r="BE10">
+        <v>0</v>
+      </c>
+      <c r="BF10">
+        <v>0</v>
+      </c>
+      <c r="BG10">
+        <v>0</v>
+      </c>
+      <c r="BH10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2054,18 +2263,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1593DC-037F-4A85-BABE-2E6BDEE01A44}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2108,6 +2317,20 @@
       </c>
       <c r="C5" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>100003</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2249,7 +2472,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:AZ1048576"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2290,7 +2513,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2342,7 +2565,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AJ1" sqref="E1:AJ1048576"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
REaranged some things and added two materials
</commit_message>
<xml_diff>
--- a/Material classification.xlsx
+++ b/Material classification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TCCMaterialLibrary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E28BF2-D3C0-4439-A02F-5EFA62D520E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA504B5-DA19-4531-816F-F1A8D57A6736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="816" activeTab="2" xr2:uid="{6F2A3154-DBF6-40E9-8E64-C416931478F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="816" activeTab="1" xr2:uid="{6F2A3154-DBF6-40E9-8E64-C416931478F8}"/>
   </bookViews>
   <sheets>
     <sheet name="ID creation" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="79">
   <si>
     <t>METALS AND ALLOYS</t>
   </si>
@@ -249,80 +249,6 @@
   </si>
   <si>
     <t>Emissivity at RT</t>
-  </si>
-  <si>
-    <r>
-      <t>LaCoO</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>La</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0.7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Sr</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0.3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CoO</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
   </si>
   <si>
     <t>La0.7Sr0.3CoO3</t>
@@ -350,7 +276,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,14 +300,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1018,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F6D9E-7E96-474D-8137-0B481F54EEF6}">
   <dimension ref="A1:BH10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D10"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AK8" sqref="AK8:BH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2057,10 +1975,178 @@
         <v>200001</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+      <c r="AG8">
+        <v>1</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>0</v>
+      </c>
+      <c r="AV8">
+        <v>0</v>
+      </c>
+      <c r="AW8">
+        <v>0</v>
+      </c>
+      <c r="AX8">
+        <v>0</v>
+      </c>
+      <c r="AY8">
+        <v>0</v>
+      </c>
+      <c r="AZ8">
+        <v>0</v>
+      </c>
+      <c r="BA8">
+        <v>0</v>
+      </c>
+      <c r="BB8">
+        <v>0</v>
+      </c>
+      <c r="BC8">
+        <v>0</v>
+      </c>
+      <c r="BD8">
+        <v>0</v>
+      </c>
+      <c r="BE8">
+        <v>0</v>
+      </c>
+      <c r="BF8">
+        <v>0</v>
+      </c>
+      <c r="BG8">
+        <v>0</v>
+      </c>
+      <c r="BH8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:60" x14ac:dyDescent="0.25">
@@ -2068,10 +2154,178 @@
         <v>200002</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>1</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>0</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>0</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+      <c r="AT9">
+        <v>0</v>
+      </c>
+      <c r="AU9">
+        <v>0</v>
+      </c>
+      <c r="AV9">
+        <v>0</v>
+      </c>
+      <c r="AW9">
+        <v>0</v>
+      </c>
+      <c r="AX9">
+        <v>0</v>
+      </c>
+      <c r="AY9">
+        <v>0</v>
+      </c>
+      <c r="AZ9">
+        <v>0</v>
+      </c>
+      <c r="BA9">
+        <v>0</v>
+      </c>
+      <c r="BB9">
+        <v>0</v>
+      </c>
+      <c r="BC9">
+        <v>0</v>
+      </c>
+      <c r="BD9">
+        <v>0</v>
+      </c>
+      <c r="BE9">
+        <v>0</v>
+      </c>
+      <c r="BF9">
+        <v>0</v>
+      </c>
+      <c r="BG9">
+        <v>0</v>
+      </c>
+      <c r="BH9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:60" x14ac:dyDescent="0.25">
@@ -2079,13 +2333,13 @@
         <v>100003</v>
       </c>
       <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" t="s">
         <v>78</v>
-      </c>
-      <c r="C10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" t="s">
-        <v>80</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2265,7 +2519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1593DC-037F-4A85-BABE-2E6BDEE01A44}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -2324,13 +2578,13 @@
         <v>100003</v>
       </c>
       <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" t="s">
         <v>78</v>
-      </c>
-      <c r="C6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2343,14 +2597,14 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2379,7 +2633,10 @@
         <v>200001</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.35">
@@ -2388,6 +2645,9 @@
       </c>
       <c r="B5" t="s">
         <v>73</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Ag and BeO, moved some files from appInfos
</commit_message>
<xml_diff>
--- a/Material classification.xlsx
+++ b/Material classification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TCCMaterialLibrary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA09D732-A97B-4FD1-B281-4F83C0920D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD2D8BE-35F9-48DE-AD57-7C8A67C09439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="816" activeTab="1" xr2:uid="{6F2A3154-DBF6-40E9-8E64-C416931478F8}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="106">
   <si>
     <t>METALS AND ALLOYS</t>
   </si>
@@ -479,6 +479,18 @@
   </si>
   <si>
     <t>Nitinol</t>
+  </si>
+  <si>
+    <t>BeO</t>
+  </si>
+  <si>
+    <t>Berillium oxide</t>
+  </si>
+  <si>
+    <t>Ag</t>
+  </si>
+  <si>
+    <t>Silver</t>
   </si>
 </sst>
 </file>
@@ -1157,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F6D9E-7E96-474D-8137-0B481F54EEF6}">
-  <dimension ref="A1:BI19"/>
+  <dimension ref="A1:BI21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AV19" sqref="AV19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4417,6 +4429,370 @@
         <v>0</v>
       </c>
     </row>
+    <row r="20" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>100005</v>
+      </c>
+      <c r="B20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>1</v>
+      </c>
+      <c r="AA20">
+        <v>1</v>
+      </c>
+      <c r="AB20">
+        <v>1</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <v>1</v>
+      </c>
+      <c r="AG20">
+        <v>1</v>
+      </c>
+      <c r="AH20">
+        <v>1</v>
+      </c>
+      <c r="AI20">
+        <v>0</v>
+      </c>
+      <c r="AJ20">
+        <v>0</v>
+      </c>
+      <c r="AK20">
+        <v>0</v>
+      </c>
+      <c r="AL20">
+        <v>0</v>
+      </c>
+      <c r="AM20">
+        <v>0</v>
+      </c>
+      <c r="AN20">
+        <v>0</v>
+      </c>
+      <c r="AO20">
+        <v>0</v>
+      </c>
+      <c r="AP20">
+        <v>0</v>
+      </c>
+      <c r="AQ20">
+        <v>0</v>
+      </c>
+      <c r="AR20">
+        <v>0</v>
+      </c>
+      <c r="AS20">
+        <v>0</v>
+      </c>
+      <c r="AT20">
+        <v>0</v>
+      </c>
+      <c r="AU20">
+        <v>0</v>
+      </c>
+      <c r="AV20">
+        <v>0</v>
+      </c>
+      <c r="AW20">
+        <v>0</v>
+      </c>
+      <c r="AX20">
+        <v>0</v>
+      </c>
+      <c r="AY20">
+        <v>0</v>
+      </c>
+      <c r="AZ20">
+        <v>0</v>
+      </c>
+      <c r="BA20">
+        <v>0</v>
+      </c>
+      <c r="BB20">
+        <v>0</v>
+      </c>
+      <c r="BC20">
+        <v>0</v>
+      </c>
+      <c r="BD20">
+        <v>0</v>
+      </c>
+      <c r="BE20">
+        <v>0</v>
+      </c>
+      <c r="BF20">
+        <v>0</v>
+      </c>
+      <c r="BG20">
+        <v>0</v>
+      </c>
+      <c r="BH20">
+        <v>0</v>
+      </c>
+      <c r="BI20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>200005</v>
+      </c>
+      <c r="B21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>1</v>
+      </c>
+      <c r="Z21">
+        <v>1</v>
+      </c>
+      <c r="AA21">
+        <v>1</v>
+      </c>
+      <c r="AB21">
+        <v>1</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
+        <v>1</v>
+      </c>
+      <c r="AG21">
+        <v>1</v>
+      </c>
+      <c r="AH21">
+        <v>1</v>
+      </c>
+      <c r="AI21">
+        <v>0</v>
+      </c>
+      <c r="AJ21">
+        <v>0</v>
+      </c>
+      <c r="AK21">
+        <v>0</v>
+      </c>
+      <c r="AL21">
+        <v>0</v>
+      </c>
+      <c r="AM21">
+        <v>0</v>
+      </c>
+      <c r="AN21">
+        <v>0</v>
+      </c>
+      <c r="AO21">
+        <v>0</v>
+      </c>
+      <c r="AP21">
+        <v>0</v>
+      </c>
+      <c r="AQ21">
+        <v>0</v>
+      </c>
+      <c r="AR21">
+        <v>0</v>
+      </c>
+      <c r="AS21">
+        <v>0</v>
+      </c>
+      <c r="AT21">
+        <v>0</v>
+      </c>
+      <c r="AU21">
+        <v>0</v>
+      </c>
+      <c r="AV21">
+        <v>0</v>
+      </c>
+      <c r="AW21">
+        <v>0</v>
+      </c>
+      <c r="AX21">
+        <v>0</v>
+      </c>
+      <c r="AY21">
+        <v>0</v>
+      </c>
+      <c r="AZ21">
+        <v>0</v>
+      </c>
+      <c r="BA21">
+        <v>0</v>
+      </c>
+      <c r="BB21">
+        <v>0</v>
+      </c>
+      <c r="BC21">
+        <v>0</v>
+      </c>
+      <c r="BD21">
+        <v>0</v>
+      </c>
+      <c r="BE21">
+        <v>0</v>
+      </c>
+      <c r="BF21">
+        <v>0</v>
+      </c>
+      <c r="BG21">
+        <v>0</v>
+      </c>
+      <c r="BH21">
+        <v>0</v>
+      </c>
+      <c r="BI21">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4424,10 +4800,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1593DC-037F-4A85-BABE-2E6BDEE01A44}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4505,6 +4881,17 @@
         <v>101</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>100005</v>
+      </c>
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4512,10 +4899,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543E0AFA-6024-4581-9565-D9A221BC4139}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4580,6 +4967,20 @@
       </c>
       <c r="D6" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>200004</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added two columns to excel
</commit_message>
<xml_diff>
--- a/Material classification.xlsx
+++ b/Material classification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TCCbuilder Dropbox\Katja Vozel\KATJA LAHDE PRIVATE\TCCbuilder\TCCbuilder library\Prepared materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TCCMaterialLibrary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A94D62A-27A4-4431-8F62-25062F1C5B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D16424-318D-4A27-859C-4CF56A3F9491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="816" activeTab="1" xr2:uid="{6F2A3154-DBF6-40E9-8E64-C416931478F8}"/>
+    <workbookView xWindow="-25320" yWindow="390" windowWidth="25440" windowHeight="15390" tabRatio="816" activeTab="1" xr2:uid="{6F2A3154-DBF6-40E9-8E64-C416931478F8}"/>
   </bookViews>
   <sheets>
     <sheet name="ID creation" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="96">
   <si>
     <t>METALS AND ALLOYS</t>
   </si>
@@ -499,6 +499,24 @@
   </si>
   <si>
     <t>Dimensionality</t>
+  </si>
+  <si>
+    <t>Phase at RT</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Therm. conductor</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
@@ -615,7 +633,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -629,7 +647,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1147,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F6D9E-7E96-474D-8137-0B481F54EEF6}">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,18 +1177,20 @@
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="14.28515625" customWidth="1"/>
-    <col min="16" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="14.28515625" customWidth="1"/>
+    <col min="18" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>88</v>
       </c>
@@ -1190,100 +1209,111 @@
       <c r="F1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
-        <f>FLOOR(C2/100000, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="B2" s="9">
-        <f>FLOOR((C2-A2*100000)/10000,1)</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="9">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f t="shared" ref="A2:A24" si="0">FLOOR(C2/100000, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B24" si="1">FLOOR((C2-A2*100000)/10000,1)</f>
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>100001</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9">
-        <v>1</v>
-      </c>
-      <c r="H2" s="9">
-        <v>0</v>
-      </c>
-      <c r="I2" s="9">
-        <v>0</v>
-      </c>
-      <c r="J2" s="9">
-        <v>0</v>
-      </c>
-      <c r="K2" s="9">
-        <v>0</v>
-      </c>
-      <c r="L2" s="9">
-        <v>0</v>
-      </c>
-      <c r="M2" s="9">
-        <v>0</v>
-      </c>
-      <c r="N2" s="9">
-        <v>0</v>
-      </c>
-      <c r="O2" s="9">
-        <v>0</v>
-      </c>
-      <c r="P2" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>FLOOR(C3/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B3">
-        <f>FLOOR((C3-A3*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C3">
@@ -1295,20 +1325,20 @@
       <c r="E3" t="s">
         <v>31</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
+      <c r="G3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" t="s">
+        <v>93</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1326,69 +1356,80 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <f>FLOOR(C4/100000, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="9">
-        <f>FLOOR((C4-A4*100000)/10000,1)</f>
-        <v>1</v>
-      </c>
-      <c r="C4" s="9">
+      <c r="B4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>310001</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9" t="s">
+      <c r="F4" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="9">
-        <v>0</v>
-      </c>
-      <c r="H4" s="9">
-        <v>0</v>
-      </c>
-      <c r="I4" s="9">
-        <v>0</v>
-      </c>
-      <c r="J4" s="9">
-        <v>1</v>
-      </c>
-      <c r="K4" s="9">
-        <v>0</v>
-      </c>
-      <c r="L4" s="9">
-        <v>0</v>
-      </c>
-      <c r="M4" s="9">
-        <v>0</v>
-      </c>
-      <c r="N4" s="9">
-        <v>0</v>
-      </c>
-      <c r="O4" s="9">
-        <v>0</v>
-      </c>
-      <c r="P4" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>FLOOR(C5/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B5">
-        <f>FLOOR((C5-A5*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C5">
@@ -1400,14 +1441,14 @@
       <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
+      <c r="G5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" t="s">
+        <v>93</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1433,14 +1474,20 @@
       <c r="Q5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>FLOOR(C6/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B6">
-        <f>FLOOR((C6-A6*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C6">
@@ -1452,14 +1499,14 @@
       <c r="E6" t="s">
         <v>40</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
+      <c r="G6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" t="s">
+        <v>93</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1485,14 +1532,20 @@
       <c r="Q6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>FLOOR(C7/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B7">
-        <f>FLOOR((C7-A7*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C7">
@@ -1504,14 +1557,14 @@
       <c r="E7" t="s">
         <v>38</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
+      <c r="G7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" t="s">
+        <v>93</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1537,14 +1590,20 @@
       <c r="Q7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>FLOOR(C8/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B8">
-        <f>FLOOR((C8-A8*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C8">
@@ -1559,20 +1618,20 @@
       <c r="F8" t="s">
         <v>43</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
+      <c r="G8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" t="s">
+        <v>93</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1590,16 +1649,22 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A9">
-        <f>FLOOR(C9/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B9">
-        <f>FLOOR((C9-A9*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C9">
@@ -1614,17 +1679,17 @@
       <c r="F9" t="s">
         <v>48</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
+      <c r="G9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" t="s">
+        <v>93</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -1647,14 +1712,20 @@
       <c r="Q9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A10">
-        <f>FLOOR(C10/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B10">
-        <f>FLOOR((C10-A10*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C10">
@@ -1669,17 +1740,17 @@
       <c r="F10" t="s">
         <v>48</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
+      <c r="G10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" t="s">
+        <v>93</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1702,14 +1773,20 @@
       <c r="Q10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A11">
-        <f>FLOOR(C11/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B11">
-        <f>FLOOR((C11-A11*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C11">
@@ -1724,17 +1801,17 @@
       <c r="F11" t="s">
         <v>48</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
+      <c r="G11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" t="s">
+        <v>93</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1757,14 +1834,20 @@
       <c r="Q11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>FLOOR(C12/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B12">
-        <f>FLOOR((C12-A12*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C12">
@@ -1779,17 +1862,17 @@
       <c r="F12" t="s">
         <v>52</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
+      <c r="G12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" t="s">
+        <v>93</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -1801,25 +1884,31 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>FLOOR(C13/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B13">
-        <f>FLOOR((C13-A13*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C13">
@@ -1831,14 +1920,14 @@
       <c r="E13" t="s">
         <v>54</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
+      <c r="G13" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" t="s">
+        <v>93</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1864,14 +1953,20 @@
       <c r="Q13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A14">
-        <f>FLOOR(C14/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B14">
-        <f>FLOOR((C14-A14*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C14">
@@ -1886,14 +1981,14 @@
       <c r="F14" t="s">
         <v>58</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
+      <c r="G14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" t="s">
+        <v>93</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1919,14 +2014,20 @@
       <c r="Q14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A15">
-        <f>FLOOR(C15/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B15">
-        <f>FLOOR((C15-A15*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C15">
@@ -1941,14 +2042,14 @@
       <c r="F15" t="s">
         <v>61</v>
       </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
+      <c r="G15" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" t="s">
+        <v>93</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1974,14 +2075,20 @@
       <c r="Q15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>FLOOR(C16/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B16">
-        <f>FLOOR((C16-A16*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C16">
@@ -1996,14 +2103,14 @@
       <c r="F16" t="s">
         <v>63</v>
       </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
+      <c r="G16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" t="s">
+        <v>95</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -2029,14 +2136,20 @@
       <c r="Q16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>FLOOR(C17/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B17">
-        <f>FLOOR((C17-A17*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C17">
@@ -2048,29 +2161,29 @@
       <c r="E17" t="s">
         <v>66</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
+      <c r="G17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" t="s">
+        <v>93</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -2081,14 +2194,20 @@
       <c r="Q17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>FLOOR(C18/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B18">
-        <f>FLOOR((C18-A18*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C18">
@@ -2100,14 +2219,14 @@
       <c r="E18" t="s">
         <v>70</v>
       </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
+      <c r="G18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18" t="s">
+        <v>93</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -2133,14 +2252,20 @@
       <c r="Q18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>FLOOR(C19/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B19">
-        <f>FLOOR((C19-A19*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C19">
@@ -2152,14 +2277,14 @@
       <c r="E19" t="s">
         <v>67</v>
       </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
+      <c r="G19" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" t="s">
+        <v>93</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -2185,14 +2310,20 @@
       <c r="Q19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>FLOOR(C20/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B20">
-        <f>FLOOR((C20-A20*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C20">
@@ -2204,23 +2335,23 @@
       <c r="F20" t="s">
         <v>72</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
+      <c r="G20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" t="s">
+        <v>93</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -2237,14 +2368,20 @@
       <c r="Q20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A21">
-        <f>FLOOR(C21/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B21">
-        <f>FLOOR((C21-A21*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C21">
@@ -2259,14 +2396,14 @@
       <c r="F21" t="s">
         <v>74</v>
       </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
+      <c r="G21" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" t="s">
+        <v>93</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -2292,14 +2429,20 @@
       <c r="Q21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>FLOOR(C22/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B22">
-        <f>FLOOR((C22-A22*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C22">
@@ -2311,14 +2454,14 @@
       <c r="F22" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
+      <c r="G22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" t="s">
+        <v>93</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -2344,14 +2487,20 @@
       <c r="Q22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>FLOOR(C23/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B23">
-        <f>FLOOR((C23-A23*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C23">
@@ -2363,14 +2512,14 @@
       <c r="E23" t="s">
         <v>79</v>
       </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
+      <c r="G23" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" t="s">
+        <v>93</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23">
         <v>0</v>
@@ -2396,14 +2545,20 @@
       <c r="Q23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>FLOOR(C24/100000, 1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B24">
-        <f>FLOOR((C24-A24*100000)/10000,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C24">
@@ -2418,14 +2573,14 @@
       <c r="F24" t="s">
         <v>85</v>
       </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
+      <c r="G24" t="s">
+        <v>91</v>
+      </c>
+      <c r="H24" t="s">
+        <v>93</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -2449,6 +2604,12 @@
         <v>0</v>
       </c>
       <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrected flags - I hope they are correct now
</commit_message>
<xml_diff>
--- a/Material classification.xlsx
+++ b/Material classification.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TCCbuilder Dropbox\Katja Vozel\KATJA LAHDE PRIVATE\TCCbuilder\TCCbuilder library\Prepared materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TCCbuilder Dropbox\Katja Vozel\KATJA LAHDE PRIVATE\TCCbuilder\TCCbuilder library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8411A2E4-60FA-410F-93C0-D29DC519983B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F85847-B0F5-444D-829B-9E3DFEF5EE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="816" activeTab="8" xr2:uid="{6F2A3154-DBF6-40E9-8E64-C416931478F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="816" activeTab="1" xr2:uid="{6F2A3154-DBF6-40E9-8E64-C416931478F8}"/>
   </bookViews>
   <sheets>
     <sheet name="ID creation" sheetId="1" r:id="rId1"/>
     <sheet name="MATERIALS" sheetId="9" r:id="rId2"/>
-    <sheet name="METALS AND ALLOYS" sheetId="2" r:id="rId3"/>
-    <sheet name="CERAMICS" sheetId="3" r:id="rId4"/>
-    <sheet name="POLYMERS" sheetId="4" r:id="rId5"/>
-    <sheet name="COMPOSITES" sheetId="5" r:id="rId6"/>
-    <sheet name="SEMICONDUCTORS" sheetId="6" r:id="rId7"/>
-    <sheet name="BIOMATERIALS" sheetId="7" r:id="rId8"/>
-    <sheet name="OTHER" sheetId="8" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId4"/>
+    <sheet name="METALS AND ALLOYS" sheetId="2" r:id="rId5"/>
+    <sheet name="CERAMICS" sheetId="3" r:id="rId6"/>
+    <sheet name="POLYMERS" sheetId="4" r:id="rId7"/>
+    <sheet name="COMPOSITES" sheetId="5" r:id="rId8"/>
+    <sheet name="SEMICONDUCTORS" sheetId="6" r:id="rId9"/>
+    <sheet name="BIOMATERIALS" sheetId="7" r:id="rId10"/>
+    <sheet name="OTHER" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1175,7 +1177,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1262,9 +1264,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1302,7 +1304,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1408,7 +1410,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1550,7 +1552,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1691,13 +1693,333 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A5A395-2BE1-4735-8205-D880D9FF88DC}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADFEE978-670C-45C2-8B8E-2685CC2B68F4}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>700001</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>700002</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>700003</v>
+      </c>
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>700004</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>700005</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>700006</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <v>700007</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>700008</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>700008</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <v>700009</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="9">
+        <v>700010</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="9">
+        <v>700011</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>710012</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>700013</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>700014</v>
+      </c>
+      <c r="B19" t="s">
+        <v>191</v>
+      </c>
+      <c r="C19" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>700015</v>
+      </c>
+      <c r="B20" t="s">
+        <v>193</v>
+      </c>
+      <c r="C20" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>700016</v>
+      </c>
+      <c r="B21" t="s">
+        <v>194</v>
+      </c>
+      <c r="C21" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>700017</v>
+      </c>
+      <c r="B22" t="s">
+        <v>195</v>
+      </c>
+      <c r="C22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>700018</v>
+      </c>
+      <c r="B23" t="s">
+        <v>196</v>
+      </c>
+      <c r="C23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>700019</v>
+      </c>
+      <c r="B24" t="s">
+        <v>198</v>
+      </c>
+      <c r="C24" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>700020</v>
+      </c>
+      <c r="B25" t="s">
+        <v>204</v>
+      </c>
+      <c r="C25" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>700021</v>
+      </c>
+      <c r="B26" t="s">
+        <v>206</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F6D9E-7E96-474D-8137-0B481F54EEF6}">
   <dimension ref="A1:T89"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T18" sqref="T18"/>
+      <selection pane="bottomLeft" activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,14 +2032,16 @@
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="14.28515625" customWidth="1"/>
-    <col min="18" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1750,31 +2074,31 @@
         <v>17</v>
       </c>
       <c r="J1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>19</v>
       </c>
       <c r="M1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="P1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="S1" s="7" t="s">
         <v>81</v>
@@ -1875,13 +2199,13 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -2183,13 +2507,13 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -2244,10 +2568,10 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -2308,10 +2632,10 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -2372,10 +2696,10 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -2436,10 +2760,10 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -2454,13 +2778,13 @@
         <v>0</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12">
         <v>0</v>
@@ -2530,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -2750,10 +3074,10 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -2762,10 +3086,10 @@
         <v>0</v>
       </c>
       <c r="N17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -3060,10 +3384,10 @@
       <c r="J22">
         <v>0</v>
       </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
       <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
         <v>0</v>
       </c>
       <c r="N22">
@@ -4830,10 +5154,10 @@
         <v>0</v>
       </c>
       <c r="J51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L51">
         <v>0</v>
@@ -4848,10 +5172,10 @@
         <v>0</v>
       </c>
       <c r="P51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R51">
         <v>0</v>
@@ -4894,10 +5218,10 @@
         <v>0</v>
       </c>
       <c r="J52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L52">
         <v>0</v>
@@ -4958,10 +5282,10 @@
         <v>0</v>
       </c>
       <c r="J53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L53">
         <v>0</v>
@@ -5022,10 +5346,10 @@
         <v>0</v>
       </c>
       <c r="J54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L54">
         <v>0</v>
@@ -5040,10 +5364,10 @@
         <v>0</v>
       </c>
       <c r="P54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R54">
         <v>0</v>
@@ -5086,10 +5410,10 @@
         <v>0</v>
       </c>
       <c r="J55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L55">
         <v>0</v>
@@ -5104,10 +5428,10 @@
         <v>0</v>
       </c>
       <c r="P55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R55">
         <v>0</v>
@@ -5150,10 +5474,10 @@
         <v>0</v>
       </c>
       <c r="J56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L56">
         <v>0</v>
@@ -5168,10 +5492,10 @@
         <v>0</v>
       </c>
       <c r="P56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R56">
         <v>0</v>
@@ -5214,10 +5538,10 @@
         <v>0</v>
       </c>
       <c r="J57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L57">
         <v>0</v>
@@ -5226,10 +5550,10 @@
         <v>0</v>
       </c>
       <c r="N57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P57">
         <v>0</v>
@@ -5278,10 +5602,10 @@
         <v>0</v>
       </c>
       <c r="J58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L58">
         <v>0</v>
@@ -5339,10 +5663,10 @@
         <v>0</v>
       </c>
       <c r="J59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L59">
         <v>0</v>
@@ -5357,10 +5681,10 @@
         <v>0</v>
       </c>
       <c r="P59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R59">
         <v>0</v>
@@ -5705,10 +6029,10 @@
         <v>0</v>
       </c>
       <c r="J65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L65">
         <v>0</v>
@@ -5726,10 +6050,10 @@
         <v>1</v>
       </c>
       <c r="Q65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S65">
         <v>0</v>
@@ -6196,10 +6520,10 @@
         <v>0</v>
       </c>
       <c r="J73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L73">
         <v>0</v>
@@ -6257,10 +6581,10 @@
         <v>0</v>
       </c>
       <c r="J74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L74">
         <v>0</v>
@@ -6318,10 +6642,10 @@
         <v>0</v>
       </c>
       <c r="J75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L75">
         <v>0</v>
@@ -6379,10 +6703,10 @@
         <v>0</v>
       </c>
       <c r="J76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L76">
         <v>0</v>
@@ -6440,10 +6764,10 @@
         <v>0</v>
       </c>
       <c r="J77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L77">
         <v>0</v>
@@ -6510,19 +6834,19 @@
         <v>0</v>
       </c>
       <c r="M78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O78">
         <v>0</v>
       </c>
       <c r="P78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R78">
         <v>0</v>
@@ -6571,19 +6895,19 @@
         <v>0</v>
       </c>
       <c r="M79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O79">
         <v>0</v>
       </c>
       <c r="P79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R79">
         <v>0</v>
@@ -6632,19 +6956,19 @@
         <v>0</v>
       </c>
       <c r="M80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O80">
         <v>0</v>
       </c>
       <c r="P80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R80">
         <v>0</v>
@@ -6693,19 +7017,19 @@
         <v>0</v>
       </c>
       <c r="M81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O81">
         <v>0</v>
       </c>
       <c r="P81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R81">
         <v>0</v>
@@ -6754,19 +7078,19 @@
         <v>0</v>
       </c>
       <c r="M82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O82">
         <v>0</v>
       </c>
       <c r="P82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R82">
         <v>0</v>
@@ -6815,19 +7139,19 @@
         <v>0</v>
       </c>
       <c r="M83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O83">
         <v>0</v>
       </c>
       <c r="P83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R83">
         <v>0</v>
@@ -6870,13 +7194,13 @@
         <v>0</v>
       </c>
       <c r="K84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L84">
         <v>0</v>
       </c>
       <c r="M84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N84">
         <v>0</v>
@@ -6931,13 +7255,13 @@
         <v>0</v>
       </c>
       <c r="K85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L85">
         <v>0</v>
       </c>
       <c r="M85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N85">
         <v>0</v>
@@ -6992,13 +7316,13 @@
         <v>0</v>
       </c>
       <c r="K86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L86">
         <v>0</v>
       </c>
       <c r="M86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N86">
         <v>0</v>
@@ -7056,13 +7380,13 @@
         <v>0</v>
       </c>
       <c r="K87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L87">
         <v>0</v>
       </c>
       <c r="M87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N87">
         <v>0</v>
@@ -7120,13 +7444,13 @@
         <v>0</v>
       </c>
       <c r="K88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L88">
         <v>0</v>
       </c>
       <c r="M88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N88">
         <v>0</v>
@@ -7184,13 +7508,13 @@
         <v>0</v>
       </c>
       <c r="K89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L89">
         <v>0</v>
       </c>
       <c r="M89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N89">
         <v>0</v>
@@ -7220,6 +7544,836 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D83C26-A5C8-49CB-8017-4B620E99931C}">
+  <dimension ref="A1:K65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F809C2-320A-4573-891D-2B32BB2DB803}">
+  <dimension ref="A1:K65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1593DC-037F-4A85-BABE-2E6BDEE01A44}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -7695,7 +8849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543E0AFA-6024-4581-9565-D9A221BC4139}">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -7909,7 +9063,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA21FC2-010F-4D0F-9D28-FD434D616E24}">
   <dimension ref="A1:D34"/>
   <sheetViews>
@@ -8063,7 +9217,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED095D1F-5EE4-4B2F-ABDB-409DF804549D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -8118,7 +9272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DFB59B1-E19D-4D9C-8B98-AEC1652D5DBD}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -8273,324 +9427,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A5A395-2BE1-4735-8205-D880D9FF88DC}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADFEE978-670C-45C2-8B8E-2685CC2B68F4}">
-  <dimension ref="A1:D26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>700001</v>
-      </c>
-      <c r="B5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>700002</v>
-      </c>
-      <c r="B6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>700003</v>
-      </c>
-      <c r="B7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>700004</v>
-      </c>
-      <c r="B8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <v>700005</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>700006</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="9">
-        <v>700007</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>700008</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="9">
-        <v>700008</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="9">
-        <v>700009</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="9">
-        <v>700010</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="9">
-        <v>700011</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>710012</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
-        <v>700013</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
-        <v>700014</v>
-      </c>
-      <c r="B19" t="s">
-        <v>191</v>
-      </c>
-      <c r="C19" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
-        <v>700015</v>
-      </c>
-      <c r="B20" t="s">
-        <v>193</v>
-      </c>
-      <c r="C20" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
-        <v>700016</v>
-      </c>
-      <c r="B21" t="s">
-        <v>194</v>
-      </c>
-      <c r="C21" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
-        <v>700017</v>
-      </c>
-      <c r="B22" t="s">
-        <v>195</v>
-      </c>
-      <c r="C22" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>700018</v>
-      </c>
-      <c r="B23" t="s">
-        <v>196</v>
-      </c>
-      <c r="C23" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
-        <v>700019</v>
-      </c>
-      <c r="B24" t="s">
-        <v>198</v>
-      </c>
-      <c r="C24" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
-        <v>700020</v>
-      </c>
-      <c r="B25" t="s">
-        <v>204</v>
-      </c>
-      <c r="C25" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
-        <v>700021</v>
-      </c>
-      <c r="B26" t="s">
-        <v>206</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>207</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected some more errors
</commit_message>
<xml_diff>
--- a/Material classification.xlsx
+++ b/Material classification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TCCMaterialLibrary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5CFCF6-FF5C-413A-A01F-6D3E3ADF7A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F3125F-5BD9-45DA-A010-75D9813CA905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="816" activeTab="1" xr2:uid="{6F2A3154-DBF6-40E9-8E64-C416931478F8}"/>
+    <workbookView xWindow="1350" yWindow="1530" windowWidth="21840" windowHeight="12510" tabRatio="816" activeTab="5" xr2:uid="{6F2A3154-DBF6-40E9-8E64-C416931478F8}"/>
   </bookViews>
   <sheets>
     <sheet name="ID creation" sheetId="1" r:id="rId1"/>
@@ -276,12 +276,6 @@
   </si>
   <si>
     <t>PFH-O</t>
-  </si>
-  <si>
-    <t>paraffin-polystyrene foam hybrid</t>
-  </si>
-  <si>
-    <t>made with octadecane</t>
   </si>
   <si>
     <t>kThysteresis</t>
@@ -1114,6 +1108,12 @@
       </rPr>
       <t xml:space="preserve"> Bismuth telluride</t>
     </r>
+  </si>
+  <si>
+    <t>made with octadecane, porous</t>
+  </si>
+  <si>
+    <t>Paraffin-polystyrene foam hybrid</t>
   </si>
 </sst>
 </file>
@@ -1778,9 +1778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F6D9E-7E96-474D-8137-0B481F54EEF6}">
   <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L97" sqref="L97"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1808,10 +1808,10 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>23</v>
@@ -1826,10 +1826,10 @@
         <v>16</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>17</v>
@@ -1838,7 +1838,7 @@
         <v>22</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>19</v>
@@ -1859,13 +1859,13 @@
         <v>31</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="T1" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1887,10 +1887,10 @@
         <v>25</v>
       </c>
       <c r="G2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" t="s">
         <v>86</v>
-      </c>
-      <c r="H2" t="s">
-        <v>88</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1948,10 +1948,10 @@
         <v>27</v>
       </c>
       <c r="G3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" t="s">
         <v>86</v>
-      </c>
-      <c r="H3" t="s">
-        <v>88</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2006,16 +2006,16 @@
         <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F4" t="s">
         <v>33</v>
       </c>
       <c r="G4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" t="s">
         <v>86</v>
-      </c>
-      <c r="H4" t="s">
-        <v>88</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -2073,10 +2073,10 @@
         <v>29</v>
       </c>
       <c r="G5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" t="s">
         <v>86</v>
-      </c>
-      <c r="H5" t="s">
-        <v>88</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -2134,10 +2134,10 @@
         <v>36</v>
       </c>
       <c r="G6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" t="s">
         <v>86</v>
-      </c>
-      <c r="H6" t="s">
-        <v>88</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -2195,10 +2195,10 @@
         <v>34</v>
       </c>
       <c r="G7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" t="s">
         <v>86</v>
-      </c>
-      <c r="H7" t="s">
-        <v>88</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -2253,16 +2253,16 @@
         <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F8" t="s">
         <v>39</v>
       </c>
       <c r="G8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" t="s">
         <v>86</v>
-      </c>
-      <c r="H8" t="s">
-        <v>88</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -2323,10 +2323,10 @@
         <v>44</v>
       </c>
       <c r="G9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" t="s">
         <v>86</v>
-      </c>
-      <c r="H9" t="s">
-        <v>88</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -2387,10 +2387,10 @@
         <v>44</v>
       </c>
       <c r="G10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" t="s">
         <v>86</v>
-      </c>
-      <c r="H10" t="s">
-        <v>88</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -2451,10 +2451,10 @@
         <v>44</v>
       </c>
       <c r="G11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" t="s">
         <v>86</v>
-      </c>
-      <c r="H11" t="s">
-        <v>88</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -2509,16 +2509,16 @@
         <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>226</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>225</v>
       </c>
       <c r="G12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" t="s">
         <v>86</v>
-      </c>
-      <c r="H12" t="s">
-        <v>88</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -2570,16 +2570,16 @@
         <v>300002</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" t="s">
         <v>86</v>
-      </c>
-      <c r="H13" t="s">
-        <v>88</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -2631,19 +2631,19 @@
         <v>200003</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" t="s">
         <v>86</v>
-      </c>
-      <c r="H14" t="s">
-        <v>88</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -2695,19 +2695,19 @@
         <v>510005</v>
       </c>
       <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
         <v>54</v>
       </c>
-      <c r="E15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" t="s">
-        <v>56</v>
-      </c>
       <c r="G15" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" t="s">
         <v>86</v>
-      </c>
-      <c r="H15" t="s">
-        <v>88</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -2759,19 +2759,19 @@
         <v>500006</v>
       </c>
       <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" t="s">
         <v>57</v>
       </c>
-      <c r="E16" t="s">
-        <v>59</v>
-      </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -2823,16 +2823,16 @@
         <v>100004</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" t="s">
         <v>86</v>
-      </c>
-      <c r="H17" t="s">
-        <v>88</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -2884,16 +2884,16 @@
         <v>100005</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" t="s">
         <v>86</v>
-      </c>
-      <c r="H18" t="s">
-        <v>88</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -2945,16 +2945,16 @@
         <v>200005</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G19" t="s">
+        <v>84</v>
+      </c>
+      <c r="H19" t="s">
         <v>86</v>
-      </c>
-      <c r="H19" t="s">
-        <v>88</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -3006,19 +3006,19 @@
         <v>310003</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G20" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20" t="s">
         <v>86</v>
-      </c>
-      <c r="H20" t="s">
-        <v>88</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -3070,19 +3070,19 @@
         <v>200005</v>
       </c>
       <c r="D21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" t="s">
         <v>68</v>
       </c>
-      <c r="E21" t="s">
-        <v>70</v>
-      </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G21" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21" t="s">
         <v>86</v>
-      </c>
-      <c r="H21" t="s">
-        <v>88</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -3134,16 +3134,16 @@
         <v>100006</v>
       </c>
       <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F22" s="8" t="s">
-        <v>73</v>
-      </c>
       <c r="G22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -3192,16 +3192,16 @@
         <v>300004</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G23" t="s">
+        <v>84</v>
+      </c>
+      <c r="H23" t="s">
         <v>86</v>
-      </c>
-      <c r="H23" t="s">
-        <v>88</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -3253,19 +3253,19 @@
         <v>310005</v>
       </c>
       <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" t="s">
         <v>78</v>
       </c>
-      <c r="E24" t="s">
-        <v>79</v>
-      </c>
-      <c r="F24" t="s">
-        <v>80</v>
-      </c>
       <c r="G24" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" t="s">
         <v>86</v>
-      </c>
-      <c r="H24" t="s">
-        <v>88</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -3317,16 +3317,16 @@
         <v>700001</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
       </c>
       <c r="G25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -3378,16 +3378,16 @@
         <v>700002</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
       </c>
       <c r="G26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I26">
         <v>1</v>
@@ -3439,16 +3439,16 @@
         <v>700003</v>
       </c>
       <c r="D27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
       </c>
       <c r="G27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I27">
         <v>1</v>
@@ -3500,16 +3500,16 @@
         <v>700004</v>
       </c>
       <c r="D28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E28" t="s">
         <v>13</v>
       </c>
       <c r="G28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I28">
         <v>1</v>
@@ -3561,16 +3561,16 @@
         <v>100007</v>
       </c>
       <c r="D29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I29">
         <v>1</v>
@@ -3622,16 +3622,16 @@
         <v>100008</v>
       </c>
       <c r="D30" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G30" t="s">
+        <v>84</v>
+      </c>
+      <c r="H30" t="s">
         <v>86</v>
-      </c>
-      <c r="H30" t="s">
-        <v>88</v>
       </c>
       <c r="I30">
         <v>1</v>
@@ -3683,16 +3683,16 @@
         <v>100009</v>
       </c>
       <c r="D31" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G31" t="s">
+        <v>84</v>
+      </c>
+      <c r="H31" t="s">
         <v>86</v>
-      </c>
-      <c r="H31" t="s">
-        <v>88</v>
       </c>
       <c r="I31">
         <v>1</v>
@@ -3744,16 +3744,16 @@
         <v>100010</v>
       </c>
       <c r="D32" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E32" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I32">
         <v>1</v>
@@ -3805,16 +3805,16 @@
         <v>100011</v>
       </c>
       <c r="D33" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G33" t="s">
+        <v>84</v>
+      </c>
+      <c r="H33" t="s">
         <v>86</v>
-      </c>
-      <c r="H33" t="s">
-        <v>88</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -3866,16 +3866,16 @@
         <v>100012</v>
       </c>
       <c r="D34" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E34" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G34" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -3927,16 +3927,16 @@
         <v>100013</v>
       </c>
       <c r="D35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E35" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G35" t="s">
+        <v>84</v>
+      </c>
+      <c r="H35" t="s">
         <v>86</v>
-      </c>
-      <c r="H35" t="s">
-        <v>88</v>
       </c>
       <c r="I35">
         <v>1</v>
@@ -3988,16 +3988,16 @@
         <v>500007</v>
       </c>
       <c r="D36" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H36" t="s">
         <v>86</v>
-      </c>
-      <c r="H36" t="s">
-        <v>88</v>
       </c>
       <c r="I36">
         <v>1</v>
@@ -4049,16 +4049,16 @@
         <v>100014</v>
       </c>
       <c r="D37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G37" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I37">
         <v>1</v>
@@ -4110,16 +4110,16 @@
         <v>100015</v>
       </c>
       <c r="D38" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E38" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G38" t="s">
+        <v>84</v>
+      </c>
+      <c r="H38" t="s">
         <v>86</v>
-      </c>
-      <c r="H38" t="s">
-        <v>88</v>
       </c>
       <c r="I38">
         <v>1</v>
@@ -4171,16 +4171,16 @@
         <v>100016</v>
       </c>
       <c r="D39" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G39" t="s">
+        <v>84</v>
+      </c>
+      <c r="H39" t="s">
         <v>86</v>
-      </c>
-      <c r="H39" t="s">
-        <v>88</v>
       </c>
       <c r="I39">
         <v>1</v>
@@ -4232,16 +4232,16 @@
         <v>100017</v>
       </c>
       <c r="D40" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E40" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G40" t="s">
+        <v>84</v>
+      </c>
+      <c r="H40" t="s">
         <v>86</v>
-      </c>
-      <c r="H40" t="s">
-        <v>88</v>
       </c>
       <c r="I40">
         <v>1</v>
@@ -4293,16 +4293,16 @@
         <v>100018</v>
       </c>
       <c r="D41" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E41" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G41" t="s">
+        <v>84</v>
+      </c>
+      <c r="H41" t="s">
         <v>86</v>
-      </c>
-      <c r="H41" t="s">
-        <v>88</v>
       </c>
       <c r="I41">
         <v>1</v>
@@ -4354,16 +4354,16 @@
         <v>700005</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G42" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I42">
         <v>1</v>
@@ -4415,16 +4415,16 @@
         <v>700006</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I43">
         <v>1</v>
@@ -4476,16 +4476,16 @@
         <v>700007</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I44">
         <v>1</v>
@@ -4537,16 +4537,16 @@
         <v>700008</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G45" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I45">
         <v>1</v>
@@ -4598,16 +4598,16 @@
         <v>700008</v>
       </c>
       <c r="D46" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E46" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="E46" s="9" t="s">
-        <v>130</v>
-      </c>
       <c r="G46" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I46">
         <v>1</v>
@@ -4659,16 +4659,16 @@
         <v>700009</v>
       </c>
       <c r="D47" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E47" t="s">
         <v>129</v>
       </c>
-      <c r="E47" t="s">
-        <v>131</v>
-      </c>
       <c r="G47" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I47">
         <v>1</v>
@@ -4720,16 +4720,16 @@
         <v>700010</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E48" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G48" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I48">
         <v>1</v>
@@ -4781,16 +4781,16 @@
         <v>700011</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G49" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I49">
         <v>1</v>
@@ -4842,16 +4842,16 @@
         <v>710012</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G50" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I50">
         <v>1</v>
@@ -4903,19 +4903,19 @@
         <v>100019</v>
       </c>
       <c r="D51" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F51" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G51" t="s">
+        <v>84</v>
+      </c>
+      <c r="H51" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H51" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I51">
         <v>0</v>
@@ -4967,19 +4967,19 @@
         <v>100020</v>
       </c>
       <c r="D52" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E52" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F52" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G52" t="s">
+        <v>84</v>
+      </c>
+      <c r="H52" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H52" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I52">
         <v>0</v>
@@ -5031,19 +5031,19 @@
         <v>100021</v>
       </c>
       <c r="D53" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E53" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F53" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G53" t="s">
+        <v>84</v>
+      </c>
+      <c r="H53" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H53" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I53">
         <v>0</v>
@@ -5095,19 +5095,19 @@
         <v>100022</v>
       </c>
       <c r="D54" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E54" t="s">
+        <v>142</v>
+      </c>
+      <c r="F54" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="F54" s="8" t="s">
-        <v>146</v>
-      </c>
       <c r="G54" t="s">
+        <v>84</v>
+      </c>
+      <c r="H54" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I54">
         <v>0</v>
@@ -5159,19 +5159,19 @@
         <v>100023</v>
       </c>
       <c r="D55" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E55" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G55" t="s">
+        <v>84</v>
+      </c>
+      <c r="H55" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H55" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I55">
         <v>0</v>
@@ -5223,19 +5223,19 @@
         <v>100024</v>
       </c>
       <c r="D56" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E56" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G56" t="s">
+        <v>84</v>
+      </c>
+      <c r="H56" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H56" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I56">
         <v>0</v>
@@ -5287,19 +5287,19 @@
         <v>100025</v>
       </c>
       <c r="D57" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E57" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G57" t="s">
+        <v>84</v>
+      </c>
+      <c r="H57" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H57" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I57">
         <v>0</v>
@@ -5351,19 +5351,19 @@
         <v>110026</v>
       </c>
       <c r="D58" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E58" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F58" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G58" t="s">
+        <v>84</v>
+      </c>
+      <c r="H58" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H58" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I58">
         <v>0</v>
@@ -5415,16 +5415,16 @@
         <v>120027</v>
       </c>
       <c r="D59" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E59" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G59" t="s">
+        <v>84</v>
+      </c>
+      <c r="H59" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H59" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I59">
         <v>0</v>
@@ -5473,19 +5473,19 @@
         <v>310006</v>
       </c>
       <c r="D60" t="s">
+        <v>157</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="F60" t="s">
+        <v>156</v>
+      </c>
+      <c r="G60" t="s">
+        <v>84</v>
+      </c>
+      <c r="H60" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="F60" t="s">
-        <v>158</v>
-      </c>
-      <c r="G60" t="s">
-        <v>86</v>
-      </c>
-      <c r="H60" s="9" t="s">
-        <v>161</v>
       </c>
       <c r="I60">
         <v>0</v>
@@ -5537,16 +5537,16 @@
         <v>300007</v>
       </c>
       <c r="D61" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E61" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G61" t="s">
+        <v>84</v>
+      </c>
+      <c r="H61" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H61" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I61">
         <v>1</v>
@@ -5598,16 +5598,16 @@
         <v>700013</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G62" t="s">
+        <v>84</v>
+      </c>
+      <c r="H62" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H62" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I62">
         <v>1</v>
@@ -5659,16 +5659,16 @@
         <v>500008</v>
       </c>
       <c r="D63" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E63" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G63" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H63" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I63">
         <v>1</v>
@@ -5720,16 +5720,16 @@
         <v>500009</v>
       </c>
       <c r="D64" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E64" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G64" t="s">
+        <v>84</v>
+      </c>
+      <c r="H64" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H64" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I64">
         <v>1</v>
@@ -5781,16 +5781,16 @@
         <v>100028</v>
       </c>
       <c r="D65" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E65" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G65" t="s">
+        <v>84</v>
+      </c>
+      <c r="H65" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H65" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I65">
         <v>0</v>
@@ -5842,16 +5842,16 @@
         <v>200007</v>
       </c>
       <c r="D66" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E66" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G66" t="s">
+        <v>84</v>
+      </c>
+      <c r="H66" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H66" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I66">
         <v>1</v>
@@ -5903,19 +5903,19 @@
         <v>200009</v>
       </c>
       <c r="D67" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E67" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F67" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G67" t="s">
+        <v>84</v>
+      </c>
+      <c r="H67" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H67" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I67">
         <v>1</v>
@@ -5967,16 +5967,16 @@
         <v>200010</v>
       </c>
       <c r="D68" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E68" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G68" t="s">
+        <v>84</v>
+      </c>
+      <c r="H68" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H68" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I68">
         <v>1</v>
@@ -6028,16 +6028,16 @@
         <v>200011</v>
       </c>
       <c r="D69" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E69" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G69" t="s">
+        <v>84</v>
+      </c>
+      <c r="H69" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H69" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I69">
         <v>1</v>
@@ -6089,16 +6089,16 @@
         <v>200012</v>
       </c>
       <c r="D70" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E70" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G70" t="s">
+        <v>84</v>
+      </c>
+      <c r="H70" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H70" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I70">
         <v>1</v>
@@ -6150,16 +6150,16 @@
         <v>200013</v>
       </c>
       <c r="D71" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E71" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G71" t="s">
+        <v>84</v>
+      </c>
+      <c r="H71" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H71" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I71">
         <v>1</v>
@@ -6211,16 +6211,16 @@
         <v>200014</v>
       </c>
       <c r="D72" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E72" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G72" t="s">
+        <v>84</v>
+      </c>
+      <c r="H72" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H72" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I72">
         <v>0</v>
@@ -6272,16 +6272,16 @@
         <v>700014</v>
       </c>
       <c r="D73" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G73" t="s">
+        <v>84</v>
+      </c>
+      <c r="H73" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H73" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I73">
         <v>0</v>
@@ -6333,16 +6333,16 @@
         <v>700015</v>
       </c>
       <c r="D74" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G74" t="s">
+        <v>84</v>
+      </c>
+      <c r="H74" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H74" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I74">
         <v>0</v>
@@ -6394,16 +6394,16 @@
         <v>700016</v>
       </c>
       <c r="D75" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G75" t="s">
+        <v>84</v>
+      </c>
+      <c r="H75" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H75" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I75">
         <v>0</v>
@@ -6455,16 +6455,16 @@
         <v>700017</v>
       </c>
       <c r="D76" t="s">
+        <v>193</v>
+      </c>
+      <c r="E76" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="E76" s="8" t="s">
-        <v>197</v>
-      </c>
       <c r="G76" t="s">
+        <v>84</v>
+      </c>
+      <c r="H76" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H76" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I76">
         <v>0</v>
@@ -6516,16 +6516,16 @@
         <v>700018</v>
       </c>
       <c r="D77" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G77" t="s">
+        <v>84</v>
+      </c>
+      <c r="H77" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H77" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I77">
         <v>0</v>
@@ -6577,16 +6577,16 @@
         <v>700019</v>
       </c>
       <c r="D78" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E78" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G78" t="s">
+        <v>84</v>
+      </c>
+      <c r="H78" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H78" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I78">
         <v>0</v>
@@ -6638,16 +6638,16 @@
         <v>300008</v>
       </c>
       <c r="D79" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E79" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G79" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H79" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I79">
         <v>0</v>
@@ -6699,16 +6699,16 @@
         <v>100029</v>
       </c>
       <c r="D80" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E80" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G80" t="s">
+        <v>84</v>
+      </c>
+      <c r="H80" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H80" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I80">
         <v>0</v>
@@ -6760,16 +6760,16 @@
         <v>100030</v>
       </c>
       <c r="D81" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E81" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G81" t="s">
+        <v>84</v>
+      </c>
+      <c r="H81" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H81" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I81">
         <v>0</v>
@@ -6821,16 +6821,16 @@
         <v>700020</v>
       </c>
       <c r="D82" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E82" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G82" t="s">
+        <v>84</v>
+      </c>
+      <c r="H82" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H82" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I82">
         <v>0</v>
@@ -6882,16 +6882,16 @@
         <v>700021</v>
       </c>
       <c r="D83" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G83" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H83" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I83">
         <v>0</v>
@@ -6943,16 +6943,16 @@
         <v>100031</v>
       </c>
       <c r="D84" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E84" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G84" t="s">
+        <v>84</v>
+      </c>
+      <c r="H84" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H84" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I84">
         <v>0</v>
@@ -7004,16 +7004,16 @@
         <v>100032</v>
       </c>
       <c r="D85" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E85" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G85" t="s">
+        <v>84</v>
+      </c>
+      <c r="H85" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H85" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I85">
         <v>0</v>
@@ -7065,16 +7065,16 @@
         <v>100033</v>
       </c>
       <c r="D86" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E86" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G86" t="s">
+        <v>84</v>
+      </c>
+      <c r="H86" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H86" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I86">
         <v>0</v>
@@ -7126,19 +7126,19 @@
         <v>100034</v>
       </c>
       <c r="D87" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E87" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F87" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G87" t="s">
+        <v>84</v>
+      </c>
+      <c r="H87" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H87" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I87">
         <v>0</v>
@@ -7190,19 +7190,19 @@
         <v>100035</v>
       </c>
       <c r="D88" t="s">
+        <v>208</v>
+      </c>
+      <c r="E88" t="s">
+        <v>208</v>
+      </c>
+      <c r="F88" t="s">
         <v>210</v>
       </c>
-      <c r="E88" t="s">
-        <v>210</v>
-      </c>
-      <c r="F88" t="s">
-        <v>212</v>
-      </c>
       <c r="G88" t="s">
+        <v>84</v>
+      </c>
+      <c r="H88" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H88" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I88">
         <v>0</v>
@@ -7254,19 +7254,19 @@
         <v>100036</v>
       </c>
       <c r="D89" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E89" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F89" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G89" t="s">
+        <v>84</v>
+      </c>
+      <c r="H89" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H89" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I89">
         <v>0</v>
@@ -7318,16 +7318,16 @@
         <v>200015</v>
       </c>
       <c r="D90" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E90" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G90" t="s">
+        <v>84</v>
+      </c>
+      <c r="H90" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H90" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I90">
         <v>1</v>
@@ -7379,16 +7379,16 @@
         <v>200016</v>
       </c>
       <c r="D91" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E91" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G91" t="s">
+        <v>84</v>
+      </c>
+      <c r="H91" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H91" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I91">
         <v>1</v>
@@ -7440,16 +7440,16 @@
         <v>200017</v>
       </c>
       <c r="D92" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E92" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G92" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H92" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I92">
         <v>1</v>
@@ -7501,16 +7501,16 @@
         <v>500010</v>
       </c>
       <c r="D93" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E93" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G93" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H93" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I93">
         <v>1</v>
@@ -7562,19 +7562,19 @@
         <v>310009</v>
       </c>
       <c r="D94" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E94" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F94" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G94" t="s">
+        <v>84</v>
+      </c>
+      <c r="H94" t="s">
         <v>86</v>
-      </c>
-      <c r="H94" t="s">
-        <v>88</v>
       </c>
       <c r="I94">
         <v>0</v>
@@ -7626,19 +7626,19 @@
         <v>500011</v>
       </c>
       <c r="D95" t="s">
+        <v>222</v>
+      </c>
+      <c r="E95" t="s">
         <v>224</v>
       </c>
-      <c r="E95" t="s">
-        <v>226</v>
-      </c>
       <c r="F95" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G95" t="s">
+        <v>84</v>
+      </c>
+      <c r="H95" t="s">
         <v>86</v>
-      </c>
-      <c r="H95" t="s">
-        <v>88</v>
       </c>
       <c r="I95">
         <v>0</v>
@@ -7748,7 +7748,7 @@
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
         <v>39</v>
@@ -7759,10 +7759,10 @@
         <v>100004</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -7770,10 +7770,10 @@
         <v>100005</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -7781,13 +7781,13 @@
         <v>100006</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -7795,10 +7795,10 @@
         <v>100007</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7806,10 +7806,10 @@
         <v>100008</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -7817,10 +7817,10 @@
         <v>100009</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7828,10 +7828,10 @@
         <v>100010</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -7839,10 +7839,10 @@
         <v>100011</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -7850,10 +7850,10 @@
         <v>100012</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -7861,10 +7861,10 @@
         <v>100013</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -7872,10 +7872,10 @@
         <v>100014</v>
       </c>
       <c r="B17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -7883,10 +7883,10 @@
         <v>100015</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -7894,10 +7894,10 @@
         <v>100016</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -7905,10 +7905,10 @@
         <v>100017</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -7916,10 +7916,10 @@
         <v>100018</v>
       </c>
       <c r="B21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -7927,13 +7927,13 @@
         <v>100019</v>
       </c>
       <c r="B22" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -7941,13 +7941,13 @@
         <v>100020</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -7955,13 +7955,13 @@
         <v>100021</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -7969,13 +7969,13 @@
         <v>100022</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -7983,13 +7983,13 @@
         <v>100023</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -7997,13 +7997,13 @@
         <v>100024</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D27" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -8011,13 +8011,13 @@
         <v>100025</v>
       </c>
       <c r="B28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -8025,13 +8025,13 @@
         <v>110026</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -8039,10 +8039,10 @@
         <v>120027</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -8050,10 +8050,10 @@
         <v>100028</v>
       </c>
       <c r="B31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C31" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -8061,10 +8061,10 @@
         <v>100029</v>
       </c>
       <c r="B32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -8072,10 +8072,10 @@
         <v>100030</v>
       </c>
       <c r="B33" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C33" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -8083,10 +8083,10 @@
         <v>100031</v>
       </c>
       <c r="B34" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C34" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -8094,10 +8094,10 @@
         <v>100032</v>
       </c>
       <c r="B35" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C35" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -8105,10 +8105,10 @@
         <v>100033</v>
       </c>
       <c r="B36" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C36" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -8116,13 +8116,13 @@
         <v>100034</v>
       </c>
       <c r="B37" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C37" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D37" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -8130,13 +8130,13 @@
         <v>100035</v>
       </c>
       <c r="B38" t="s">
+        <v>208</v>
+      </c>
+      <c r="C38" t="s">
+        <v>208</v>
+      </c>
+      <c r="D38" t="s">
         <v>210</v>
-      </c>
-      <c r="C38" t="s">
-        <v>210</v>
-      </c>
-      <c r="D38" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -8144,13 +8144,13 @@
         <v>100036</v>
       </c>
       <c r="B39" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C39" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D39" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -8221,13 +8221,13 @@
         <v>200003</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -8235,10 +8235,10 @@
         <v>200004</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.35">
@@ -8246,13 +8246,13 @@
         <v>200005</v>
       </c>
       <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
         <v>68</v>
       </c>
-      <c r="C8" t="s">
-        <v>70</v>
-      </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -8260,10 +8260,10 @@
         <v>200006</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.35">
@@ -8271,13 +8271,13 @@
         <v>200007</v>
       </c>
       <c r="B10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" t="s">
         <v>171</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>173</v>
-      </c>
-      <c r="D10" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
@@ -8285,13 +8285,13 @@
         <v>200008</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -8299,13 +8299,13 @@
         <v>200009</v>
       </c>
       <c r="B12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -8313,10 +8313,10 @@
         <v>200010</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -8324,13 +8324,13 @@
         <v>200011</v>
       </c>
       <c r="B14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" t="s">
         <v>184</v>
-      </c>
-      <c r="C14" t="s">
-        <v>185</v>
-      </c>
-      <c r="D14" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -8338,10 +8338,10 @@
         <v>200012</v>
       </c>
       <c r="B15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -8349,10 +8349,10 @@
         <v>200013</v>
       </c>
       <c r="B16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -8360,10 +8360,10 @@
         <v>200014</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -8371,10 +8371,10 @@
         <v>200015</v>
       </c>
       <c r="B18" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -8382,10 +8382,10 @@
         <v>200016</v>
       </c>
       <c r="B19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -8393,10 +8393,10 @@
         <v>200017</v>
       </c>
       <c r="B20" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C20" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -8457,10 +8457,10 @@
         <v>300002</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -8468,13 +8468,13 @@
         <v>310003</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -8482,10 +8482,10 @@
         <v>300004</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -8493,13 +8493,13 @@
         <v>310005</v>
       </c>
       <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
         <v>78</v>
-      </c>
-      <c r="C8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -8507,13 +8507,13 @@
         <v>310006</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -8521,10 +8521,10 @@
         <v>300007</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -8532,10 +8532,10 @@
         <v>300008</v>
       </c>
       <c r="B11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -8543,13 +8543,13 @@
         <v>310009</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -8580,8 +8580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED095D1F-5EE4-4B2F-ABDB-409DF804549D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8589,7 +8589,7 @@
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -8620,10 +8620,10 @@
         <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>226</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -8725,13 +8725,13 @@
         <v>510005</v>
       </c>
       <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
         <v>54</v>
-      </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -8739,13 +8739,13 @@
         <v>500006</v>
       </c>
       <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
         <v>57</v>
       </c>
-      <c r="C10" t="s">
-        <v>59</v>
-      </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -8753,10 +8753,10 @@
         <v>500007</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -8764,10 +8764,10 @@
         <v>500008</v>
       </c>
       <c r="B12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -8775,10 +8775,10 @@
         <v>500009</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -8786,10 +8786,10 @@
         <v>500010</v>
       </c>
       <c r="B14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.35">
@@ -8797,13 +8797,13 @@
         <v>500011</v>
       </c>
       <c r="B15" t="s">
+        <v>222</v>
+      </c>
+      <c r="C15" t="s">
         <v>224</v>
       </c>
-      <c r="C15" t="s">
-        <v>226</v>
-      </c>
       <c r="D15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -8890,7 +8890,7 @@
         <v>700001</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -8901,7 +8901,7 @@
         <v>700002</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -8912,7 +8912,7 @@
         <v>700003</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -8923,7 +8923,7 @@
         <v>700004</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
@@ -8934,10 +8934,10 @@
         <v>700005</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -8945,10 +8945,10 @@
         <v>700006</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
@@ -8956,10 +8956,10 @@
         <v>700007</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -8967,10 +8967,10 @@
         <v>700008</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.35">
@@ -8978,10 +8978,10 @@
         <v>700008</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.35">
@@ -8989,10 +8989,10 @@
         <v>700009</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" t="s">
         <v>129</v>
-      </c>
-      <c r="C14" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.35">
@@ -9000,10 +9000,10 @@
         <v>700010</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.35">
@@ -9011,10 +9011,10 @@
         <v>700011</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -9022,10 +9022,10 @@
         <v>710012</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -9033,10 +9033,10 @@
         <v>700013</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -9044,10 +9044,10 @@
         <v>700014</v>
       </c>
       <c r="B19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -9055,10 +9055,10 @@
         <v>700015</v>
       </c>
       <c r="B20" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -9066,10 +9066,10 @@
         <v>700016</v>
       </c>
       <c r="B21" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -9077,10 +9077,10 @@
         <v>700017</v>
       </c>
       <c r="B22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -9088,10 +9088,10 @@
         <v>700018</v>
       </c>
       <c r="B23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -9099,10 +9099,10 @@
         <v>700019</v>
       </c>
       <c r="B24" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C24" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -9110,10 +9110,10 @@
         <v>700020</v>
       </c>
       <c r="B25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C25" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -9121,10 +9121,10 @@
         <v>700021</v>
       </c>
       <c r="B26" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added graphite AXM 5Q
</commit_message>
<xml_diff>
--- a/Material classification.xlsx
+++ b/Material classification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TCCMaterialLibrary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9311CD5D-ADFD-4E05-859B-82DAE6544FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859EF0E9-12B3-452B-A0C3-A3A61990D11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="816" activeTab="1" xr2:uid="{6F2A3154-DBF6-40E9-8E64-C416931478F8}"/>
+    <workbookView xWindow="60" yWindow="855" windowWidth="21840" windowHeight="12510" tabRatio="816" activeTab="1" xr2:uid="{6F2A3154-DBF6-40E9-8E64-C416931478F8}"/>
   </bookViews>
   <sheets>
     <sheet name="ID creation" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="230">
   <si>
     <t>METALS AND ALLOYS</t>
   </si>
@@ -1120,6 +1120,9 @@
   </si>
   <si>
     <t>Cobalt vanadate</t>
+  </si>
+  <si>
+    <t>Graphite AXM 5Q</t>
   </si>
 </sst>
 </file>
@@ -1782,11 +1785,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F6D9E-7E96-474D-8137-0B481F54EEF6}">
-  <dimension ref="A1:T96"/>
+  <dimension ref="A1:T97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F96" sqref="F96"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U97" sqref="U97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7742,6 +7745,68 @@
         <v>0</v>
       </c>
     </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>5</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>500012</v>
+      </c>
+      <c r="D97" t="s">
+        <v>55</v>
+      </c>
+      <c r="E97" t="s">
+        <v>229</v>
+      </c>
+      <c r="F97" t="s">
+        <v>56</v>
+      </c>
+      <c r="G97" t="s">
+        <v>84</v>
+      </c>
+      <c r="H97" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I97">
+        <v>1</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97">
+        <v>0</v>
+      </c>
+      <c r="M97">
+        <v>0</v>
+      </c>
+      <c r="N97">
+        <v>0</v>
+      </c>
+      <c r="O97">
+        <v>0</v>
+      </c>
+      <c r="P97">
+        <v>0</v>
+      </c>
+      <c r="Q97">
+        <v>0</v>
+      </c>
+      <c r="R97">
+        <v>0</v>
+      </c>
+      <c r="S97">
+        <v>0</v>
+      </c>
+      <c r="T97">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7751,7 +7816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1593DC-037F-4A85-BABE-2E6BDEE01A44}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A37" sqref="A37:D39"/>
     </sheetView>
   </sheetViews>
@@ -8709,10 +8774,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DFB59B1-E19D-4D9C-8B98-AEC1652D5DBD}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:D15"/>
+      <selection activeCell="A16" sqref="A16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8880,6 +8945,20 @@
       </c>
       <c r="D15" t="s">
         <v>223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>500012</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
+        <v>229</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>